<commit_message>
write excel summary sheet.
</commit_message>
<xml_diff>
--- a/fixtures/yjk/1/OutReader.xlsx
+++ b/fixtures/yjk/1/OutReader.xlsx
@@ -5,13 +5,22 @@
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
     <sheet sheetId="1" name="汇总信息" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="含钢量汇总" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="计算参数" state="visible" r:id="rId6"/>
+    <sheet sheetId="4" name="周期" state="visible" r:id="rId7"/>
+    <sheet sheetId="5" name="内力" state="visible" r:id="rId8"/>
+    <sheet sheetId="6" name="位移角" state="visible" r:id="rId9"/>
+    <sheet sheetId="7" name="整体验算结果" state="visible" r:id="rId10"/>
+    <sheet sheetId="8" name="楼层分布数据" state="visible" r:id="rId11"/>
+    <sheet sheetId="9" name="调整系数" state="visible" r:id="rId12"/>
+    <sheet sheetId="10" name="工程量" state="visible" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
   <si>
     <t>计算结果记录表</t>
   </si>
@@ -92,6 +101,48 @@
   </si>
   <si>
     <t>周期折减系数</t>
+  </si>
+  <si>
+    <t>质量</t>
+  </si>
+  <si>
+    <t>活载质量</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>恒载质量</t>
+  </si>
+  <si>
+    <t>层间位移角</t>
+  </si>
+  <si>
+    <t>风荷载</t>
+  </si>
+  <si>
+    <t>X向</t>
+  </si>
+  <si>
+    <t>楼层</t>
+  </si>
+  <si>
+    <t>Y向</t>
+  </si>
+  <si>
+    <t>-偏心</t>
+  </si>
+  <si>
+    <t>限值</t>
+  </si>
+  <si>
+    <t>位移比</t>
+  </si>
+  <si>
+    <t>+偏心</t>
+  </si>
+  <si>
+    <t>1.2 or 1.4</t>
   </si>
 </sst>
 </file>
@@ -468,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F21"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -609,14 +660,298 @@
         <v>0.9</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>23980.664</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>198539.547</v>
+      </c>
+      <c r="F11">
+        <v>222520.219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <v>878</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>469</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14"/>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14">
+        <v>646</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>1.37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16">
+        <v>500</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17">
+        <v>1.44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>1.37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19">
+        <v>1.44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21"/>
+      <c r="F21"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="15">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B4"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="A5:B9"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add extract cross wind force.
</commit_message>
<xml_diff>
--- a/fixtures/yjk/1/OutReader.xlsx
+++ b/fixtures/yjk/1/OutReader.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>计算结果记录表</t>
   </si>
@@ -142,7 +142,10 @@
     <t>+偏心</t>
   </si>
   <si>
-    <t>1.2 or 1.4</t>
+    <t>1.2 / 1.4</t>
+  </si>
+  <si>
+    <t>层间位移比</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F26"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,13 +752,13 @@
         <v>35</v>
       </c>
       <c r="D15">
-        <v>1.37</v>
+        <v>1.13</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
       </c>
       <c r="F15">
-        <v>53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,7 +784,7 @@
         <v>33</v>
       </c>
       <c r="D17">
-        <v>1.44</v>
+        <v>1.06</v>
       </c>
       <c r="E17" t="s">
         <v>34</v>
@@ -797,13 +800,13 @@
         <v>35</v>
       </c>
       <c r="D18">
-        <v>1.37</v>
+        <v>1.16</v>
       </c>
       <c r="E18" t="s">
         <v>34</v>
       </c>
       <c r="F18">
-        <v>53</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -812,13 +815,13 @@
         <v>33</v>
       </c>
       <c r="D19">
-        <v>1.44</v>
+        <v>1.33</v>
       </c>
       <c r="E19" t="s">
         <v>34</v>
       </c>
       <c r="F19">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -843,8 +846,90 @@
       <c r="E21"/>
       <c r="F21"/>
     </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>1.44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F22">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23">
+        <v>1.37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
+        <v>1.44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25">
+        <v>1.37</v>
+      </c>
+      <c r="E25" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26"/>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="20">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:B4"/>
     <mergeCell ref="D2:F2"/>
@@ -860,6 +945,11 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="D21:F21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
write summary and summary-quantity sheet.
</commit_message>
<xml_diff>
--- a/fixtures/yjk/1/OutReader.xlsx
+++ b/fixtures/yjk/1/OutReader.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="101">
   <si>
     <t>计算结果记录表</t>
   </si>
@@ -28,7 +28,7 @@
     <t>工程信息</t>
   </si>
   <si>
-    <t>工程文件路径</t>
+    <t>工程路径</t>
   </si>
   <si>
     <t>/Users/yml/outreaderjs/fixtures/yjk/1</t>
@@ -88,13 +88,13 @@
     <t>地震烈度</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>修正后基本风压</t>
-  </si>
-  <si>
-    <t>刚性楼板假定</t>
+    <t>7(0.1g)</t>
+  </si>
+  <si>
+    <t>基本风压</t>
+  </si>
+  <si>
+    <t>楼板假定</t>
   </si>
   <si>
     <t>整体指标计算采用强刚，其它计算非强刚</t>
@@ -196,107 +196,148 @@
     <t>扭转系数Z</t>
   </si>
   <si>
-    <t>5.70</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>5.10</t>
-  </si>
-  <si>
-    <t>4.17</t>
-  </si>
-  <si>
-    <t>1.62</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>0.05</t>
-  </si>
-  <si>
-    <t>1.56</t>
-  </si>
-  <si>
-    <t>0.09</t>
-  </si>
-  <si>
-    <t>0.42</t>
-  </si>
-  <si>
-    <t>0.50</t>
-  </si>
-  <si>
-    <t>1.54</t>
-  </si>
-  <si>
-    <t>0.55</t>
-  </si>
-  <si>
-    <t>0.44</t>
-  </si>
-  <si>
     <t>周期比</t>
   </si>
   <si>
-    <t>0.73</t>
-  </si>
-  <si>
     <t>&lt;0.85</t>
   </si>
   <si>
-    <t>计算振型个数</t>
-  </si>
-  <si>
-    <t>95.00</t>
-  </si>
-  <si>
-    <t>93.08</t>
+    <t>计算振型数</t>
+  </si>
+  <si>
+    <t>振型质量参与系数</t>
   </si>
   <si>
     <t>基底剪力</t>
   </si>
   <si>
-    <t>-18342</t>
-  </si>
-  <si>
-    <t>27180</t>
-  </si>
-  <si>
-    <t>17347</t>
-  </si>
-  <si>
-    <t>16637</t>
-  </si>
-  <si>
-    <t>基底倾覆弯矩</t>
-  </si>
-  <si>
-    <t>-2433179</t>
-  </si>
-  <si>
-    <t>3536034</t>
-  </si>
-  <si>
-    <t>2309740</t>
-  </si>
-  <si>
-    <t>2095978</t>
+    <t>基底弯矩</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>结构面积</t>
+  </si>
+  <si>
+    <t>m^2</t>
+  </si>
+  <si>
+    <t>结构周期</t>
+  </si>
+  <si>
+    <t>T1/T2/T3</t>
+  </si>
+  <si>
+    <t>风/地震</t>
+  </si>
+  <si>
+    <t>底层墙厚</t>
+  </si>
+  <si>
+    <t>X/Y mm</t>
+  </si>
+  <si>
+    <t>底层柱截面</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>含量</t>
+  </si>
+  <si>
+    <t xml:space="preserve">钢筋含量
+kg/m^2</t>
+  </si>
+  <si>
+    <t>墙</t>
+  </si>
+  <si>
+    <t>柱</t>
+  </si>
+  <si>
+    <t>梁</t>
+  </si>
+  <si>
+    <t>板</t>
+  </si>
+  <si>
+    <t>合计</t>
+  </si>
+  <si>
+    <t xml:space="preserve">砼含量
+m^3/m^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">型钢含量
+kg/m^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">模板含量
+m^2/m^2</t>
+  </si>
+  <si>
+    <t>梁、板</t>
+  </si>
+  <si>
+    <t>压型钢板</t>
+  </si>
+  <si>
+    <t xml:space="preserve">涂料含量
+m^2/m^2</t>
+  </si>
+  <si>
+    <t>总量</t>
+  </si>
+  <si>
+    <t xml:space="preserve">钢筋总量
+t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">砼总量
+m^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">型钢总量
+t</t>
+  </si>
+  <si>
+    <t>单价</t>
+  </si>
+  <si>
+    <t>砼</t>
+  </si>
+  <si>
+    <t>元/m^3</t>
+  </si>
+  <si>
+    <t>钢筋</t>
+  </si>
+  <si>
+    <t>元/t</t>
+  </si>
+  <si>
+    <t>钢材</t>
+  </si>
+  <si>
+    <t>型钢</t>
+  </si>
+  <si>
+    <t>模板</t>
+  </si>
+  <si>
+    <t>元/m^2</t>
+  </si>
+  <si>
+    <t>涂料</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -304,16 +345,37 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F0FFF0"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFFF0"/>
+        <bgColor rgb="00FFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -321,12 +383,124 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,846 +842,856 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F51"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="15" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="6" width="15" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" ht="25" customHeight="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2"/>
-      <c r="C2" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="C3" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4" t="s">
+    <row r="4" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5"/>
-      <c r="C5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6" t="s">
+    <row r="6" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="7">
         <v>54</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>253.35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7" t="s">
+    <row r="7" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="7">
         <v>5</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8" t="s">
+    <row r="8" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9" t="s">
+    <row r="9" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10"/>
-      <c r="C10" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D10">
-        <v>23980.664</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="D10" s="7">
+        <v>23981</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
-      <c r="C11" t="s">
+    <row r="11" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D11">
-        <v>198539.547</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="D11" s="7">
+        <v>198540</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F11">
-        <v>222520.219</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F11" s="6">
+        <v>222520</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="7">
         <v>878</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
-      <c r="C13" t="s">
+    <row r="13" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="7">
         <v>469</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14" t="s">
+    <row r="14" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="7">
         <v>646</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
-      <c r="C15" t="s">
+    <row r="15" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <v>412</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16" t="s">
+    <row r="16" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C16"/>
-      <c r="D16">
+      <c r="C16" s="5"/>
+      <c r="D16" s="6">
         <v>500</v>
       </c>
-      <c r="E16"/>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="7">
         <v>1.06</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18" t="s">
+    <row r="18" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="7">
         <v>1.16</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19" t="s">
+    <row r="19" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7">
         <v>1.33</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
-      <c r="C20" t="s">
+    <row r="20" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="7">
         <v>1.13</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21"/>
-      <c r="B21" t="s">
+    <row r="21" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C21"/>
-      <c r="D21" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E21"/>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="7">
         <v>1.44</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23"/>
-      <c r="B23"/>
-      <c r="C23" t="s">
+    <row r="23" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="7">
         <v>1.37</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24" t="s">
+    <row r="24" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="7">
         <v>1.44</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25" t="s">
+    <row r="25" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="7">
         <v>1.37</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="6">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26" t="s">
+    <row r="26" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C26"/>
-      <c r="D26" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E26"/>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B27"/>
-      <c r="C27" t="s">
+      <c r="B27" s="4"/>
+      <c r="C27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="7">
         <v>1.121</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="6">
         <v>1.25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28" t="s">
+    <row r="28" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="7">
         <v>1.075</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="6">
         <v>1.25</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="7">
         <v>2.768</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30" t="s">
+    <row r="30" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="7">
         <v>1.878</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31"/>
-      <c r="B31" t="s">
+    <row r="31" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="7">
         <v>2.334</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32"/>
-      <c r="C32" t="s">
+    <row r="32" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="7">
         <v>1.842</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B33"/>
-      <c r="C33" t="s">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="7">
         <v>0.1295</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34"/>
-      <c r="B34"/>
-      <c r="C34" t="s">
+    <row r="34" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="7">
         <v>0.1893</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B35"/>
-      <c r="C35" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="7">
         <v>0.81</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36"/>
-      <c r="C36" t="s">
+    <row r="36" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="7">
         <v>0.83</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37"/>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
-      <c r="F37"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="37" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39"/>
-      <c r="B39">
+    <row r="39" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5">
         <v>1</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="7">
+        <v>5.7</v>
+      </c>
+      <c r="D39" s="7">
+        <v>0</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5">
+        <v>2</v>
+      </c>
+      <c r="C40" s="7">
+        <v>5.1</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5">
+        <v>3</v>
+      </c>
+      <c r="C41" s="7">
+        <v>4.17</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0</v>
+      </c>
+      <c r="F41" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5">
+        <v>4</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1.62</v>
+      </c>
+      <c r="D42" s="7">
+        <v>0.92</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="F42" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5">
+        <v>5</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1.56</v>
+      </c>
+      <c r="D43" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.42</v>
+      </c>
+      <c r="F43" s="6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5">
+        <v>6</v>
+      </c>
+      <c r="C44" s="7">
+        <v>1.54</v>
+      </c>
+      <c r="D44" s="7">
+        <v>0</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.55</v>
+      </c>
+      <c r="F44" s="6">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="45" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D39" t="s">
+      <c r="C45" s="7">
+        <v>0.73</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E45" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="F39" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40"/>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="F45" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D40" t="s">
-        <v>60</v>
-      </c>
-      <c r="E40" t="s">
-        <v>59</v>
-      </c>
-      <c r="F40" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41"/>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B46" s="4"/>
+      <c r="C46" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="7">
+        <v>95</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F46" s="6">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D41" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" t="s">
-        <v>59</v>
-      </c>
-      <c r="F41" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42"/>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B48" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="7">
+        <v>-18342</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" s="6">
+        <v>27180</v>
+      </c>
+    </row>
+    <row r="49" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D49" s="7">
+        <v>17347</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="6">
+        <v>16637</v>
+      </c>
+    </row>
+    <row r="50" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D42" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" t="s">
-        <v>65</v>
-      </c>
-      <c r="F42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43"/>
-      <c r="B43">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
-        <v>67</v>
-      </c>
-      <c r="D43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E43" t="s">
-        <v>69</v>
-      </c>
-      <c r="F43" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44"/>
-      <c r="B44">
-        <v>6</v>
-      </c>
-      <c r="C44" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" t="s">
-        <v>59</v>
-      </c>
-      <c r="E44" t="s">
-        <v>72</v>
-      </c>
-      <c r="F44" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45"/>
-      <c r="B45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" t="s">
-        <v>75</v>
-      </c>
-      <c r="D45" t="s">
-        <v>76</v>
-      </c>
-      <c r="E45" t="s">
-        <v>77</v>
-      </c>
-      <c r="F45">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B50" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B46"/>
-      <c r="D46" t="s">
-        <v>78</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="D50" s="7">
+        <v>-2433179</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F46" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="F50" s="6">
+        <v>3536034</v>
+      </c>
+    </row>
+    <row r="51" ht="20" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D48" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D51" s="12">
+        <v>2309740</v>
+      </c>
+      <c r="E51" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49"/>
-      <c r="B49" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" t="s">
-        <v>37</v>
-      </c>
-      <c r="F49" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D50" t="s">
-        <v>86</v>
-      </c>
-      <c r="E50" t="s">
-        <v>37</v>
-      </c>
-      <c r="F50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51"/>
-      <c r="B51" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" t="s">
-        <v>35</v>
-      </c>
-      <c r="D51" t="s">
-        <v>88</v>
-      </c>
-      <c r="E51" t="s">
-        <v>37</v>
-      </c>
-      <c r="F51" t="s">
-        <v>89</v>
+      <c r="F51" s="13">
+        <v>2095978</v>
       </c>
     </row>
   </sheetData>
@@ -1562,9 +1746,556 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C58"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="3" width="15" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="15">
+        <f>汇总信息!D3</f>
+      </c>
+      <c r="C1" s="15"/>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="6">
+        <f>汇总信息!F6</f>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="6">
+        <v>99713</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="6">
+        <f>汇总信息!C39 &amp; "/" &amp; 汇总信息!C40 &amp; "/" &amp; 汇总信息!C41</f>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="6">
+        <f>min(汇总信息!D12:D13) &amp; "/" &amp; min(汇总信息!D14:D15)</f>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="6">
+        <f>round(C35*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="6">
+        <f>round(C36*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="6">
+        <f>round(C37*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="6">
+        <f>round(C38*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="6">
+        <f>round(C39*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="6">
+        <f>round(C40/C3,2)</f>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="6">
+        <f>round(C41/C3,2)</f>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="6">
+        <f>round(C42/C3,2)</f>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="6">
+        <f>round(C43/C3,2)</f>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="6">
+        <f>round(C44/C3,2)</f>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="6">
+        <f>round(C45*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="6">
+        <f>round(C46*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="6">
+        <f>round(C47*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="6">
+        <f>round(C48*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="24" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="6">
+        <f>round(C49*1000/C3,2)</f>
+      </c>
+    </row>
+    <row r="25" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C28" s="6"/>
+    </row>
+    <row r="29" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+    </row>
+    <row r="35" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="6">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="36" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="6">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="37" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="6">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="6">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="39" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="6">
+        <v>3818</v>
+      </c>
+    </row>
+    <row r="40" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="6">
+        <v>14456</v>
+      </c>
+    </row>
+    <row r="41" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="6">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="42" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="6">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="43" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="B43" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="6">
+        <v>11376</v>
+      </c>
+    </row>
+    <row r="44" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="6">
+        <v>34273</v>
+      </c>
+    </row>
+    <row r="45" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="6">
+        <v>3428</v>
+      </c>
+    </row>
+    <row r="47" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="6">
+        <v>6998</v>
+      </c>
+    </row>
+    <row r="48" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="6">
+        <v>10425</v>
+      </c>
+    </row>
+    <row r="50" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+    </row>
+    <row r="51" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+    </row>
+    <row r="52" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="16">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="53" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C53" s="16">
+        <v>6500</v>
+      </c>
+    </row>
+    <row r="54" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="16">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="55" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="16">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="56" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" ht="20" customHeight="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="17">
+        <v>65.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="B51:C51"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
write parameters sheet. and fix wmass extrade bug.
</commit_message>
<xml_diff>
--- a/fixtures/yjk/1/OutReader.xlsx
+++ b/fixtures/yjk/1/OutReader.xlsx
@@ -19,8 +19,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <t xml:space="preserve">YJK：层顶嵌固
+PKPM：层底嵌固</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="138">
   <si>
     <t>计算结果记录表</t>
   </si>
@@ -331,6 +349,117 @@
   </si>
   <si>
     <t>涂料</t>
+  </si>
+  <si>
+    <t>结构总体信息</t>
+  </si>
+  <si>
+    <t>结构材料信息</t>
+  </si>
+  <si>
+    <t>结构所在地区</t>
+  </si>
+  <si>
+    <t>广东高规DBJ15-92-2013</t>
+  </si>
+  <si>
+    <t>嵌固端所在层号</t>
+  </si>
+  <si>
+    <t>裙房层数</t>
+  </si>
+  <si>
+    <t>转换层所在层号</t>
+  </si>
+  <si>
+    <t>加强层所在层号</t>
+  </si>
+  <si>
+    <t>计算控制信息</t>
+  </si>
+  <si>
+    <t>连梁刚度折减系数（地震）</t>
+  </si>
+  <si>
+    <t>连梁刚度折减系数（风）</t>
+  </si>
+  <si>
+    <t>刚性楼板假定</t>
+  </si>
+  <si>
+    <t>风荷载信息</t>
+  </si>
+  <si>
+    <t>使用指定风荷载数据</t>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>执行规范</t>
+  </si>
+  <si>
+    <t>GB50009-2012</t>
+  </si>
+  <si>
+    <t>地面粗糙度</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>修正后基本风压 (kN/m^2)</t>
+  </si>
+  <si>
+    <t>风荷载计算阻尼比</t>
+  </si>
+  <si>
+    <t>舒适度验算基本风压 (kN/m^2)</t>
+  </si>
+  <si>
+    <t>舒适度验算阻尼比</t>
+  </si>
+  <si>
+    <t>地震信息</t>
+  </si>
+  <si>
+    <t>按地震动区划图GB18306-2015计算</t>
+  </si>
+  <si>
+    <t>设计地震分组</t>
+  </si>
+  <si>
+    <t>一</t>
+  </si>
+  <si>
+    <t>场地类别</t>
+  </si>
+  <si>
+    <t>Ⅱ</t>
+  </si>
+  <si>
+    <t>特征周期</t>
+  </si>
+  <si>
+    <t>阻尼比</t>
+  </si>
+  <si>
+    <t>X向偶然偏心</t>
+  </si>
+  <si>
+    <t>Y向偶然偏心</t>
+  </si>
+  <si>
+    <t>地震影响系数最大值</t>
+  </si>
+  <si>
+    <t>罕遇地震影响系数最大值</t>
+  </si>
+  <si>
+    <t>最大附加阻尼比</t>
+  </si>
+  <si>
+    <t xml:space="preserve">调整后水平向减震系数 </t>
   </si>
 </sst>
 </file>
@@ -450,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -499,6 +628,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2303,11 +2435,309 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B38"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="20" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="18"/>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="18"/>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="6">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+    </row>
+    <row r="25" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="18"/>
+    </row>
+    <row r="26" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="6">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="31" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="32" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="33" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="6">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="35" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0.083</v>
+      </c>
+    </row>
+    <row r="36" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="6">
+        <v>0.475</v>
+      </c>
+    </row>
+    <row r="37" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="6">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
write general result sheet. and fix wmass interface wrong name.
</commit_message>
<xml_diff>
--- a/fixtures/yjk/1/OutReader.xlsx
+++ b/fixtures/yjk/1/OutReader.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="208">
   <si>
     <t>计算结果记录表</t>
   </si>
@@ -604,6 +604,90 @@
   </si>
   <si>
     <t>WY-</t>
+  </si>
+  <si>
+    <t>工程代号</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>设计人</t>
+  </si>
+  <si>
+    <t>校核人</t>
+  </si>
+  <si>
+    <t>塔属性</t>
+  </si>
+  <si>
+    <t>质量信息（t）</t>
+  </si>
+  <si>
+    <t>活载总质量</t>
+  </si>
+  <si>
+    <t>恒载总质量</t>
+  </si>
+  <si>
+    <t>附加总质量</t>
+  </si>
+  <si>
+    <t>结构总质量</t>
+  </si>
+  <si>
+    <t>地下室楼层侧向刚度比验算（剪切刚度）</t>
+  </si>
+  <si>
+    <t>地下室层号</t>
+  </si>
+  <si>
+    <t>方向/刚度</t>
+  </si>
+  <si>
+    <t>地下一层</t>
+  </si>
+  <si>
+    <t>地上一层</t>
+  </si>
+  <si>
+    <t>结构整体抗倾覆验算</t>
+  </si>
+  <si>
+    <t>抗倾覆力矩Mr</t>
+  </si>
+  <si>
+    <t>倾覆力矩Mov</t>
+  </si>
+  <si>
+    <t>比值Mr/Mov</t>
+  </si>
+  <si>
+    <t>零应力区（%）</t>
+  </si>
+  <si>
+    <t>X向风</t>
+  </si>
+  <si>
+    <t>Y向风</t>
+  </si>
+  <si>
+    <t>X地震</t>
+  </si>
+  <si>
+    <t>Y地震</t>
+  </si>
+  <si>
+    <t>结构整体稳定验算（刚重比）</t>
+  </si>
+  <si>
+    <t>风振舒适度验算（顶点加速度）</t>
+  </si>
+  <si>
+    <t>顺风向</t>
+  </si>
+  <si>
+    <t>横风向</t>
   </si>
 </sst>
 </file>
@@ -736,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -821,6 +905,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -15592,9 +15679,474 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E42"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="5" width="15" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" s="6">
+        <v>23980.664</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="6">
+        <v>198539.547</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="13">
+        <v>222520.219</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="7">
+        <v>5</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="16"/>
+      <c r="B23" s="7">
+        <v>189630000</v>
+      </c>
+      <c r="C23" s="7">
+        <v>97253000</v>
+      </c>
+      <c r="D23" s="6">
+        <v>1.9499</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="12">
+        <v>254000000</v>
+      </c>
+      <c r="C24" s="12">
+        <v>114400000</v>
+      </c>
+      <c r="D24" s="13">
+        <v>2.2203</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C27" s="7">
+        <v>3</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" s="7">
+        <v>121700000</v>
+      </c>
+      <c r="C29" s="7">
+        <v>3111000</v>
+      </c>
+      <c r="D29" s="7">
+        <v>39.12</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B30" s="7">
+        <v>69820000</v>
+      </c>
+      <c r="C30" s="7">
+        <v>4611000</v>
+      </c>
+      <c r="D30" s="7">
+        <v>15.14</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="7">
+        <v>117000000</v>
+      </c>
+      <c r="C31" s="7">
+        <v>3283000</v>
+      </c>
+      <c r="D31" s="7">
+        <v>35.63</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="12">
+        <v>67080000</v>
+      </c>
+      <c r="C32" s="12">
+        <v>3283000</v>
+      </c>
+      <c r="D32" s="12">
+        <v>20.43</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+    </row>
+    <row r="35" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
+      <c r="B35" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="7">
+        <v>6</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7">
+        <v>2.334</v>
+      </c>
+      <c r="E36" s="6">
+        <v>1.842</v>
+      </c>
+    </row>
+    <row r="37" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="12">
+        <v>6</v>
+      </c>
+      <c r="C37" s="12">
+        <v>1</v>
+      </c>
+      <c r="D37" s="12">
+        <v>2.768</v>
+      </c>
+      <c r="E37" s="13">
+        <v>1.878</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" s="7">
+        <v>0.063</v>
+      </c>
+      <c r="C41" s="6">
+        <v>0.078</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" ht="20" customHeight="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="B42" s="12">
+        <v>0.117</v>
+      </c>
+      <c r="C42" s="13">
+        <v>0.083</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A39:C39"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>

<commit_message>
write modify factor sheet.
</commit_message>
<xml_diff>
--- a/fixtures/yjk/1/OutReader.xlsx
+++ b/fixtures/yjk/1/OutReader.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="284">
   <si>
     <t>计算结果记录表</t>
   </si>
@@ -917,6 +917,18 @@
   </si>
   <si>
     <t>标准层1</t>
+  </si>
+  <si>
+    <t>薄弱层剪力</t>
+  </si>
+  <si>
+    <t>剪重比调整系数</t>
+  </si>
+  <si>
+    <t>0.2V0调整系数</t>
+  </si>
+  <si>
+    <t>放大系数</t>
   </si>
 </sst>
 </file>
@@ -16451,7 +16463,7 @@
       <c r="AK1" s="26"/>
       <c r="AL1" s="26"/>
     </row>
-    <row r="2" ht="20" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" ht="30" customHeight="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>147</v>
       </c>
@@ -22849,9 +22861,1286 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="7" width="10" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26" t="s">
+        <v>282</v>
+      </c>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>54</v>
+      </c>
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>53</v>
+      </c>
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>52</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>51</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>50</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>49</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F8" s="7">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>47</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>46</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>45</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E12" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>44</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E13" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>43</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>42</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <v>1</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F16" s="7">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>40</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>1</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>39</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F18" s="7">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>38</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>37</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F20" s="7">
+        <v>1</v>
+      </c>
+      <c r="G20" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>36</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E21" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>35</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E22" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
+      <c r="G22" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>34</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" s="7">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E23" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F23" s="7">
+        <v>1</v>
+      </c>
+      <c r="G23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>33</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E24" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F24" s="7">
+        <v>1</v>
+      </c>
+      <c r="G24" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="7">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E25" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F25" s="7">
+        <v>1</v>
+      </c>
+      <c r="G25" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>31</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E26" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>30</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>29</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E28" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F28" s="7">
+        <v>1</v>
+      </c>
+      <c r="G28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E29" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>27</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E30" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>26</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E31" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F31" s="7">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>25</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32" s="7">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E32" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>24</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E33" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>23</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E34" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F34" s="7">
+        <v>1</v>
+      </c>
+      <c r="G34" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>22</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="7">
+        <v>1</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E35" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F35" s="7">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>21</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
+      <c r="C36" s="7">
+        <v>1</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E36" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F36" s="7">
+        <v>1</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>20</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="C37" s="7">
+        <v>1</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E37" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>19</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38" s="7">
+        <v>1</v>
+      </c>
+      <c r="D38" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E38" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F38" s="7">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>18</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7">
+        <v>1</v>
+      </c>
+      <c r="D39" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E39" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F39" s="7">
+        <v>1</v>
+      </c>
+      <c r="G39" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>17</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1</v>
+      </c>
+      <c r="C40" s="7">
+        <v>1</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F40" s="7">
+        <v>1</v>
+      </c>
+      <c r="G40" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>16</v>
+      </c>
+      <c r="B41" s="5">
+        <v>1</v>
+      </c>
+      <c r="C41" s="7">
+        <v>1</v>
+      </c>
+      <c r="D41" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E41" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F41" s="7">
+        <v>1</v>
+      </c>
+      <c r="G41" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>15</v>
+      </c>
+      <c r="B42" s="5">
+        <v>1</v>
+      </c>
+      <c r="C42" s="7">
+        <v>1</v>
+      </c>
+      <c r="D42" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E42" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>14</v>
+      </c>
+      <c r="B43" s="5">
+        <v>1</v>
+      </c>
+      <c r="C43" s="7">
+        <v>1</v>
+      </c>
+      <c r="D43" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E43" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F43" s="7">
+        <v>1</v>
+      </c>
+      <c r="G43" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>13</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7">
+        <v>1</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E44" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1</v>
+      </c>
+      <c r="G44" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>12</v>
+      </c>
+      <c r="B45" s="5">
+        <v>1</v>
+      </c>
+      <c r="C45" s="7">
+        <v>1</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E45" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F45" s="7">
+        <v>1</v>
+      </c>
+      <c r="G45" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>11</v>
+      </c>
+      <c r="B46" s="5">
+        <v>1</v>
+      </c>
+      <c r="C46" s="7">
+        <v>1</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E46" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>10</v>
+      </c>
+      <c r="B47" s="5">
+        <v>1</v>
+      </c>
+      <c r="C47" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="D47" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E47" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F47" s="7">
+        <v>1</v>
+      </c>
+      <c r="G47" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>9</v>
+      </c>
+      <c r="B48" s="5">
+        <v>1</v>
+      </c>
+      <c r="C48" s="7">
+        <v>1</v>
+      </c>
+      <c r="D48" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E48" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F48" s="7">
+        <v>1</v>
+      </c>
+      <c r="G48" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>8</v>
+      </c>
+      <c r="B49" s="5">
+        <v>1</v>
+      </c>
+      <c r="C49" s="7">
+        <v>1</v>
+      </c>
+      <c r="D49" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E49" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F49" s="7">
+        <v>1</v>
+      </c>
+      <c r="G49" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>7</v>
+      </c>
+      <c r="B50" s="5">
+        <v>1</v>
+      </c>
+      <c r="C50" s="7">
+        <v>1</v>
+      </c>
+      <c r="D50" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E50" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F50" s="7">
+        <v>1</v>
+      </c>
+      <c r="G50" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>6</v>
+      </c>
+      <c r="B51" s="5">
+        <v>1</v>
+      </c>
+      <c r="C51" s="7">
+        <v>1</v>
+      </c>
+      <c r="D51" s="7">
+        <v>1.116</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1.163</v>
+      </c>
+      <c r="F51" s="7">
+        <v>1</v>
+      </c>
+      <c r="G51" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>5</v>
+      </c>
+      <c r="B52" s="5">
+        <v>1</v>
+      </c>
+      <c r="C52" s="7">
+        <v>1</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>4</v>
+      </c>
+      <c r="B53" s="5">
+        <v>1</v>
+      </c>
+      <c r="C53" s="7">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>3</v>
+      </c>
+      <c r="B54" s="5">
+        <v>1</v>
+      </c>
+      <c r="C54" s="7">
+        <v>1</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>2</v>
+      </c>
+      <c r="B55" s="5">
+        <v>1</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" ht="20" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="10">
+        <v>1</v>
+      </c>
+      <c r="B56" s="11">
+        <v>1</v>
+      </c>
+      <c r="C56" s="12">
+        <v>1</v>
+      </c>
+      <c r="D56" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E56" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56" s="12"/>
+      <c r="G56" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>